<commit_message>
Just some small changes, not significant, (i.g. formatting, change of var names).
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -15,7 +15,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">88
+B C E I n c . 
+ 2 0 1 5 A N N U A L R E PO R T
+7 Selected annual 
+and quarterly information
+7.1 Annual financial information
+The following table shows selected consolidated financial data of BCE for 2015, 2014 and 2013, prepared in accordance with IFRS as issued 
+by the International Accounting Standards Board (IASB). We discuss the factors that caused our results to vary over the past two years 
+throughout this MD&amp;A.
+2015
+2014 (1)
+2013 (2)
+CONSOLIDATED INCOME STATEMENTS
+Operating revenues
+21,514
+21,042
+20,400
+Operating costs
+(12,963)
+(12,739)
+(12,311)
+Adjusted EBITDA
+8,551
+8,303
+8,089
+Severance, acquisition and other costs
+(446)
+(216)
+(406)
+Depreciation
+(2,890)
+(2,880)
+(2,734)
+Amortization
+(530)
+(572)
+(646)
+Finance costs
+Interest expense
+(909)
+(929)
+(931)
+Interest on post-employment benefit obligations
+(110)
+(101)
+(150)
+Other (expense) income
+(12)
+42
+(6)
+Income taxes
+(924)
+(929)
+(828)
+Net earnings
+2,730
+2,718
+2,388
+Net earnings attributable to:
+Common shareholders
+2,526
+2,363
+1,975
+Preferred shareholders
+152
+137
+131
+Non-controlling interest
+52
+218
+282
+Net earnings
+2,730
+2,718
+2,388
+Net earnings per common share
+Basic
+2.98
+2.98
+2.55
+Diluted
+2.98
+2.97
+2.54
+Included in net earnings:
+Severance, acquisition and other costs
+(327)
+(148)
+(299)
+Net gains (losses) on investments
+21
+8
+(7)
+Early debt redemption costs
+(13)
+(21)
+(36)
+Adjusted net earnings
+2,845
+2,524
+2,317
+Adjusted EPS
+3.36
+3.18
+2.99
+RATIOS
+Adjusted EBITDA margin (%)
+39.7%
+39.5%
+39.7%
+Return on equity (%) (3)
+21.1%
+21.0%
+17.9%
+(1) On October 31, 2014, BCE completed its acquisition of all the issued and outstanding common shares of Bell Aliant that it did not already own. Refer to section 6.5, Privatization 
+of Bell Aliant for further details on the transaction.
+(2) On July 5, 2013, BCE acquired 100% of the issued and outstanding shares of Astral. As part of its approval of the Astral acquisition, the CRTC ordered BCE to spend $246.9 million in 
+new benefits for French- and English-language TV, radio and film content development, support for emerging Canadian musical talent, training and professional development for 
+Canadian media, and new consumer participation initiatives. The present value of this tangible benefits obligation, amounting to $230 million, was recorded as an acquisition cost in 
+Severance, acquisition and other costs in 2013. Total acquisition and other costs relating to Astral, including the tangible benefits obligation, amounted to $266 million in 2013.
+(3) Net earnings attributable to common shareholders divided by total average equity attributable to BCE shareholders excluding preferred shares.
+</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,14 +474,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>

</xml_diff>